<commit_message>
updated tract data dictionary with limitations column
</commit_message>
<xml_diff>
--- a/tractsDataDictionary.xlsx
+++ b/tractsDataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wimer\github\opioid-policy-scan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB6A841-80E2-4927-B257-9E1DB405A2D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E9A0B5-1D24-4F46-9CC0-96C7C27D7CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22943" yWindow="-14655" windowWidth="38595" windowHeight="21795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tractsDataDictionary" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="319">
   <si>
     <t>Theme</t>
   </si>
@@ -987,6 +987,9 @@
   </si>
   <si>
     <t>3*</t>
+  </si>
+  <si>
+    <t>Data Limitations</t>
   </si>
 </sst>
 </file>
@@ -1838,10 +1841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P128"/>
+  <dimension ref="A1:Q128"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1854,7 +1857,7 @@
     <col min="11" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1901,10 +1904,13 @@
         <v>8</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1929,8 +1935,11 @@
       <c r="O2" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1955,8 +1964,11 @@
       <c r="O3" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1981,8 +1993,11 @@
       <c r="O4" s="2">
         <v>36526</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -2007,8 +2022,11 @@
       <c r="O5" s="1" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -2033,8 +2051,11 @@
       <c r="O6" s="1" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -2074,8 +2095,11 @@
       <c r="O7" s="1">
         <v>9744</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -2107,8 +2131,11 @@
       <c r="O8" s="1">
         <v>9670</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -2148,8 +2175,11 @@
       <c r="O9" s="1">
         <v>4532</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -2175,8 +2205,11 @@
       <c r="O10" s="1">
         <v>5556</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -2216,8 +2249,11 @@
       <c r="O11" s="1">
         <v>80.290000000000006</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P11" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -2257,8 +2293,11 @@
       <c r="O12" s="1">
         <v>13.78</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P12" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -2298,8 +2337,11 @@
       <c r="O13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P13" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -2339,8 +2381,11 @@
       <c r="O14" s="1">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P14" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -2380,8 +2425,11 @@
       <c r="O15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="P15" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -2421,8 +2469,11 @@
       <c r="O16" s="1">
         <v>5.55</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P16" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -2462,8 +2513,11 @@
       <c r="O17" s="1">
         <v>8.18</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P17" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -2489,8 +2543,11 @@
       <c r="O18" s="1">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P18" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -2530,8 +2587,11 @@
       <c r="O19" s="1">
         <v>14.63</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P19" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -2571,8 +2631,11 @@
       <c r="O20" s="1">
         <v>66.83</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P20" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -2612,8 +2675,11 @@
       <c r="O21" s="1">
         <v>11.45</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P21" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -2653,8 +2719,11 @@
       <c r="O22" s="1">
         <v>607</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -2694,8 +2763,11 @@
       <c r="O23" s="1">
         <v>1070</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -2735,8 +2807,11 @@
       <c r="O24" s="1">
         <v>722</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -2776,8 +2851,11 @@
       <c r="O25" s="1">
         <v>704</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
@@ -2817,8 +2895,11 @@
       <c r="O26" s="1">
         <v>4835</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
@@ -2855,8 +2936,11 @@
       <c r="O27" s="1">
         <v>495</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
         <v>22</v>
       </c>
@@ -2893,8 +2977,11 @@
       <c r="O28" s="1">
         <v>531</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
         <v>22</v>
       </c>
@@ -2934,8 +3021,11 @@
       <c r="O29" s="1">
         <v>718</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
         <v>22</v>
       </c>
@@ -2975,8 +3065,11 @@
       <c r="O30" s="1">
         <v>372</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
         <v>22</v>
       </c>
@@ -3016,8 +3109,11 @@
       <c r="O31" s="1">
         <v>1116</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
         <v>22</v>
       </c>
@@ -3049,8 +3145,11 @@
       <c r="O32" s="1">
         <v>7468</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A33" s="1" t="s">
         <v>22</v>
       </c>
@@ -3090,8 +3189,11 @@
       <c r="O33" s="1">
         <v>6352</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A34" s="1" t="s">
         <v>22</v>
       </c>
@@ -3125,8 +3227,11 @@
       <c r="O34" s="1">
         <v>8.9</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P34" s="1">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
         <v>99</v>
       </c>
@@ -3166,8 +3271,11 @@
       <c r="O35" s="1">
         <v>3.78</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P35" s="1">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
         <v>22</v>
       </c>
@@ -3198,8 +3306,11 @@
       <c r="O36" s="1">
         <v>15.7</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P36" s="1">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
         <v>22</v>
       </c>
@@ -3230,8 +3341,11 @@
       <c r="O37" s="1">
         <v>4.26</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P37" s="1">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A38" s="1" t="s">
         <v>22</v>
       </c>
@@ -3262,8 +3376,11 @@
       <c r="O38" s="1">
         <v>18.39</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P38" s="1">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A39" s="1" t="s">
         <v>22</v>
       </c>
@@ -3288,8 +3405,11 @@
       <c r="O39" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P39" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A40" s="1" t="s">
         <v>22</v>
       </c>
@@ -3314,8 +3434,11 @@
       <c r="O40" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P40" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A41" s="1" t="s">
         <v>22</v>
       </c>
@@ -3340,8 +3463,11 @@
       <c r="O41" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P41" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A42" s="1" t="s">
         <v>99</v>
       </c>
@@ -3381,8 +3507,11 @@
       <c r="O42" s="1">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P42" s="1">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A43" s="1" t="s">
         <v>99</v>
       </c>
@@ -3422,8 +3551,11 @@
       <c r="O43" s="1">
         <v>14.2</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P43" s="1">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A44" s="1" t="s">
         <v>99</v>
       </c>
@@ -3448,8 +3580,11 @@
       <c r="O44" s="1">
         <v>31504</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P44" s="1">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A45" s="1" t="s">
         <v>99</v>
       </c>
@@ -3480,8 +3615,11 @@
       <c r="O45" s="1">
         <v>29969</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P45" s="1">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A46" s="1" t="s">
         <v>99</v>
       </c>
@@ -3509,8 +3647,11 @@
       <c r="O46" s="1">
         <v>9.1</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P46" s="1">
+        <v>20996</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A47" s="1" t="s">
         <v>99</v>
       </c>
@@ -3535,8 +3676,11 @@
       <c r="O47" s="1">
         <v>128</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P47" s="1">
+        <v>21010</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A48" s="1" t="s">
         <v>99</v>
       </c>
@@ -3561,8 +3705,11 @@
       <c r="O48" s="1">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P48" s="1">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A49" s="1" t="s">
         <v>99</v>
       </c>
@@ -3587,8 +3734,11 @@
       <c r="O49" s="1">
         <v>8.0299999999999994</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P49" s="1">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A50" s="1" t="s">
         <v>99</v>
       </c>
@@ -3613,8 +3763,11 @@
       <c r="O50" s="1">
         <v>16.18</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P50" s="1">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A51" s="1" t="s">
         <v>99</v>
       </c>
@@ -3639,8 +3792,11 @@
       <c r="O51" s="1">
         <v>14.7</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P51" s="1">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A52" s="1" t="s">
         <v>99</v>
       </c>
@@ -3665,8 +3821,11 @@
       <c r="O52" s="1">
         <v>15.39</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P52" s="1">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A53" s="1" t="s">
         <v>99</v>
       </c>
@@ -3691,8 +3850,11 @@
       <c r="O53" s="1">
         <v>2092</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P53" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A54" s="1" t="s">
         <v>99</v>
       </c>
@@ -3720,8 +3882,11 @@
       <c r="O54" s="1">
         <v>37.65</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P54" s="1">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A55" s="1" t="s">
         <v>124</v>
       </c>
@@ -3746,8 +3911,11 @@
       <c r="O55" s="1">
         <v>6.64</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P55" s="1">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A56" s="1" t="s">
         <v>124</v>
       </c>
@@ -3787,8 +3955,11 @@
       <c r="O56" s="1">
         <v>11.72</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P56" s="1">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A57" s="1" t="s">
         <v>124</v>
       </c>
@@ -3813,8 +3984,11 @@
       <c r="O57" s="1">
         <v>0.68</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P57" s="1">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A58" s="1" t="s">
         <v>124</v>
       </c>
@@ -3839,8 +4013,11 @@
       <c r="O58" s="1">
         <v>8.66</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P58" s="1">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A59" s="1" t="s">
         <v>124</v>
       </c>
@@ -3865,8 +4042,11 @@
       <c r="O59" s="1">
         <v>19.899999999999999</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P59" s="1">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A60" s="1" t="s">
         <v>124</v>
       </c>
@@ -3891,8 +4071,11 @@
       <c r="O60" s="1">
         <v>673.09</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P60" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A61" s="1" t="s">
         <v>124</v>
       </c>
@@ -3917,8 +4100,11 @@
       <c r="O61" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P61" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A62" s="1" t="s">
         <v>124</v>
       </c>
@@ -3943,8 +4129,11 @@
       <c r="O62" s="1">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P62" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A63" s="1" t="s">
         <v>124</v>
       </c>
@@ -3969,8 +4158,11 @@
       <c r="O63" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P63" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A64" s="1" t="s">
         <v>10</v>
       </c>
@@ -3995,8 +4187,11 @@
       <c r="O64" s="1">
         <v>6.73</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P64" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A65" s="1" t="s">
         <v>124</v>
       </c>
@@ -4021,8 +4216,11 @@
       <c r="O65" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P65" s="1">
+        <v>47162</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A66" s="1" t="s">
         <v>124</v>
       </c>
@@ -4047,8 +4245,11 @@
       <c r="O66" s="1">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P66" s="1">
+        <v>47162</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A67" s="1" t="s">
         <v>124</v>
       </c>
@@ -4073,8 +4274,11 @@
       <c r="O67" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P67" s="1">
+        <v>47162</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A68" s="1" t="s">
         <v>124</v>
       </c>
@@ -4099,8 +4303,11 @@
       <c r="O68" s="1">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P68" s="1">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A69" s="1" t="s">
         <v>124</v>
       </c>
@@ -4125,8 +4332,11 @@
       <c r="O69" s="1">
         <v>0.81</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P69" s="1">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A70" s="1" t="s">
         <v>124</v>
       </c>
@@ -4151,8 +4361,11 @@
       <c r="O70" s="1">
         <v>0.81</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P70" s="1">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A71" s="1" t="s">
         <v>124</v>
       </c>
@@ -4177,8 +4390,11 @@
       <c r="O71" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P71" s="1">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A72" s="1" t="s">
         <v>124</v>
       </c>
@@ -4203,8 +4419,11 @@
       <c r="O72" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P72" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A73" s="1" t="s">
         <v>124</v>
       </c>
@@ -4229,8 +4448,11 @@
       <c r="O73" s="1">
         <v>13.22</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P73" s="1">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A74" s="1" t="s">
         <v>124</v>
       </c>
@@ -4255,8 +4477,11 @@
       <c r="O74" s="1">
         <v>27.39</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P74" s="1">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A75" s="1" t="s">
         <v>124</v>
       </c>
@@ -4281,8 +4506,11 @@
       <c r="O75" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P75" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A76" s="1" t="s">
         <v>124</v>
       </c>
@@ -4307,8 +4535,11 @@
       <c r="O76" s="1">
         <v>18.04</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P76" s="1">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A77" s="1" t="s">
         <v>124</v>
       </c>
@@ -4333,8 +4564,11 @@
       <c r="O77" s="1">
         <v>35.340000000000003</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P77" s="1">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A78" s="1" t="s">
         <v>124</v>
       </c>
@@ -4359,8 +4593,11 @@
       <c r="O78" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="P78" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A79" s="1" t="s">
         <v>124</v>
       </c>
@@ -4385,8 +4622,11 @@
       <c r="O79" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P79" s="1">
+        <v>3643</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A80" s="1" t="s">
         <v>124</v>
       </c>
@@ -4411,8 +4651,11 @@
       <c r="O80" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P80" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A81" s="1" t="s">
         <v>124</v>
       </c>
@@ -4437,8 +4680,11 @@
       <c r="O81" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P81" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A82" s="1" t="s">
         <v>124</v>
       </c>
@@ -4463,8 +4709,11 @@
       <c r="O82" s="1">
         <v>1744.66</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P82" s="1">
+        <v>29763</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A83" s="1" t="s">
         <v>124</v>
       </c>
@@ -4489,8 +4738,11 @@
       <c r="O83" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P83" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A84" s="1" t="s">
         <v>124</v>
       </c>
@@ -4515,8 +4767,11 @@
       <c r="O84" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P84" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A85" s="1" t="s">
         <v>124</v>
       </c>
@@ -4541,8 +4796,11 @@
       <c r="O85" s="1">
         <v>-999</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P85" s="1">
+        <v>11371</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A86" s="1" t="s">
         <v>124</v>
       </c>
@@ -4567,8 +4825,11 @@
       <c r="O86" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P86" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A87" s="1" t="s">
         <v>124</v>
       </c>
@@ -4593,8 +4854,11 @@
       <c r="O87" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P87" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A88" s="1" t="s">
         <v>124</v>
       </c>
@@ -4619,8 +4883,11 @@
       <c r="O88" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P88" s="1">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A89" s="1" t="s">
         <v>124</v>
       </c>
@@ -4645,8 +4912,11 @@
       <c r="O89" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P89" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A90" s="1" t="s">
         <v>124</v>
       </c>
@@ -4671,8 +4941,11 @@
       <c r="O90" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P90" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A91" s="1" t="s">
         <v>124</v>
       </c>
@@ -4697,8 +4970,11 @@
       <c r="O91" s="1">
         <v>148.18</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P91" s="1">
+        <v>8550</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A92" s="1" t="s">
         <v>124</v>
       </c>
@@ -4723,8 +4999,11 @@
       <c r="O92" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P92" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A93" s="1" t="s">
         <v>124</v>
       </c>
@@ -4749,8 +5028,11 @@
       <c r="O93" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P93" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A94" s="1" t="s">
         <v>124</v>
       </c>
@@ -4775,8 +5057,11 @@
       <c r="O94" s="1">
         <v>165.18</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P94" s="1">
+        <v>2662</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A95" s="1" t="s">
         <v>124</v>
       </c>
@@ -4801,8 +5086,11 @@
       <c r="O95" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P95" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A96" s="1" t="s">
         <v>124</v>
       </c>
@@ -4827,8 +5115,11 @@
       <c r="O96" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P96" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A97" s="1" t="s">
         <v>124</v>
       </c>
@@ -4853,8 +5144,11 @@
       <c r="O97" s="1">
         <v>10.23</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P97" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A98" s="1" t="s">
         <v>124</v>
       </c>
@@ -4879,8 +5173,11 @@
       <c r="O98" s="1">
         <v>19.16</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P98" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A99" s="1" t="s">
         <v>124</v>
       </c>
@@ -4905,8 +5202,11 @@
       <c r="O99" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P99" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A100" s="1" t="s">
         <v>124</v>
       </c>
@@ -4931,8 +5231,11 @@
       <c r="O100" s="1">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P100" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A101" s="1" t="s">
         <v>124</v>
       </c>
@@ -4957,8 +5260,11 @@
       <c r="O101" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P101" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A102" s="1" t="s">
         <v>124</v>
       </c>
@@ -4983,8 +5289,11 @@
       <c r="O102" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P102" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A103" s="1" t="s">
         <v>124</v>
       </c>
@@ -5009,8 +5318,11 @@
       <c r="O103" s="1">
         <v>0.84</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P103" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A104" s="1" t="s">
         <v>124</v>
       </c>
@@ -5035,8 +5347,11 @@
       <c r="O104" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P104" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A105" s="1" t="s">
         <v>124</v>
       </c>
@@ -5061,8 +5376,11 @@
       <c r="O105" s="1">
         <v>58</v>
       </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P105" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A106" s="1" t="s">
         <v>124</v>
       </c>
@@ -5087,8 +5405,11 @@
       <c r="O106" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P106" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A107" s="1" t="s">
         <v>124</v>
       </c>
@@ -5113,8 +5434,11 @@
       <c r="O107" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P107" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A108" s="1" t="s">
         <v>124</v>
       </c>
@@ -5139,8 +5463,11 @@
       <c r="O108" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P108" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A109" s="1" t="s">
         <v>124</v>
       </c>
@@ -5165,8 +5492,11 @@
       <c r="O109" s="1">
         <v>4.99</v>
       </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P109" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A110" s="1" t="s">
         <v>124</v>
       </c>
@@ -5191,8 +5521,11 @@
       <c r="O110" s="1">
         <v>17.760000000000002</v>
       </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P110" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A111" s="1" t="s">
         <v>124</v>
       </c>
@@ -5217,8 +5550,11 @@
       <c r="O111" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P111" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A112" s="1" t="s">
         <v>124</v>
       </c>
@@ -5243,8 +5579,11 @@
       <c r="O112" s="1">
         <v>13.12</v>
       </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P112" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A113" s="1" t="s">
         <v>124</v>
       </c>
@@ -5269,8 +5608,11 @@
       <c r="O113" s="1">
         <v>27.39</v>
       </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P113" s="1">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A114" s="1" t="s">
         <v>124</v>
       </c>
@@ -5295,8 +5637,11 @@
       <c r="O114" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P114" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A115" s="1" t="s">
         <v>124</v>
       </c>
@@ -5321,8 +5666,11 @@
       <c r="O115" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P115" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A116" s="1" t="s">
         <v>124</v>
       </c>
@@ -5347,8 +5695,11 @@
       <c r="O116" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P116" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A117" s="1" t="s">
         <v>124</v>
       </c>
@@ -5373,8 +5724,11 @@
       <c r="O117" s="1">
         <v>133.41999999999999</v>
       </c>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P117" s="1">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A118" s="1" t="s">
         <v>124</v>
       </c>
@@ -5399,8 +5753,11 @@
       <c r="O118" s="1">
         <v>41.05</v>
       </c>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P118" s="1">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A119" s="1" t="s">
         <v>252</v>
       </c>
@@ -5425,8 +5782,11 @@
       <c r="O119" s="1">
         <v>1.17</v>
       </c>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P119" s="1">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A120" s="1" t="s">
         <v>252</v>
       </c>
@@ -5451,8 +5811,11 @@
       <c r="O120" s="1">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P120" s="1">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A121" s="1" t="s">
         <v>252</v>
       </c>
@@ -5477,8 +5840,11 @@
       <c r="O121" s="1">
         <v>-0.06</v>
       </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P121" s="1">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A122" s="1" t="s">
         <v>252</v>
       </c>
@@ -5503,8 +5869,11 @@
       <c r="O122" s="1">
         <v>0.59</v>
       </c>
-    </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P122" s="1">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A123" s="1" t="s">
         <v>252</v>
       </c>
@@ -5529,8 +5898,11 @@
       <c r="O123" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P123" s="1">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A124" s="1" t="s">
         <v>252</v>
       </c>
@@ -5555,8 +5927,11 @@
       <c r="O124" s="1">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P124" s="1">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A125" s="1" t="s">
         <v>252</v>
       </c>
@@ -5581,8 +5956,11 @@
       <c r="O125" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P125" s="1">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A126" s="1" t="s">
         <v>252</v>
       </c>
@@ -5607,8 +5985,11 @@
       <c r="O126" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P126" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A127" s="1" t="s">
         <v>252</v>
       </c>
@@ -5633,8 +6014,11 @@
       <c r="O127" s="1">
         <v>0.61</v>
       </c>
-    </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P127" s="1">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A128" s="1" t="s">
         <v>252</v>
       </c>
@@ -5658,6 +6042,9 @@
       </c>
       <c r="O128" s="1">
         <v>0.38</v>
+      </c>
+      <c r="P128" s="1">
+        <v>494</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed typo in data dictionary
</commit_message>
<xml_diff>
--- a/tractsDataDictionary.xlsx
+++ b/tractsDataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wimer\github\opioid-policy-scan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E9A0B5-1D24-4F46-9CC0-96C7C27D7CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49EC911-7B84-4EAF-B9D0-5E7CD1CB751E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22943" yWindow="-14655" windowWidth="38595" windowHeight="21795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29078" yWindow="-14558" windowWidth="23025" windowHeight="14386" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tractsDataDictionary" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="322">
   <si>
     <t>Theme</t>
   </si>
@@ -990,6 +990,15 @@
   </si>
   <si>
     <t>Data Limitations</t>
+  </si>
+  <si>
+    <t>Walking time (minutes) to nearest buprenorphine provider</t>
+  </si>
+  <si>
+    <t>Walking time (minutes) to nearest methadone provider</t>
+  </si>
+  <si>
+    <t>Walking time (minutes) to nearest naltrexone provider</t>
   </si>
 </sst>
 </file>
@@ -1844,7 +1853,7 @@
   <dimension ref="A1:Q128"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2074,6 +2083,9 @@
       <c r="F7" s="3">
         <v>4</v>
       </c>
+      <c r="G7" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H7" s="1" t="s">
         <v>23</v>
       </c>
@@ -2228,6 +2240,9 @@
       <c r="F11" s="3">
         <v>4</v>
       </c>
+      <c r="G11" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H11" s="1" t="s">
         <v>34</v>
       </c>
@@ -2272,6 +2287,9 @@
       <c r="F12" s="3">
         <v>4</v>
       </c>
+      <c r="G12" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H12" s="1" t="s">
         <v>36</v>
       </c>
@@ -2316,6 +2334,9 @@
       <c r="F13" s="3">
         <v>4</v>
       </c>
+      <c r="G13" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H13" s="1" t="s">
         <v>38</v>
       </c>
@@ -2360,6 +2381,9 @@
       <c r="F14" s="3">
         <v>4</v>
       </c>
+      <c r="G14" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H14" s="1" t="s">
         <v>40</v>
       </c>
@@ -2404,6 +2428,9 @@
       <c r="F15" s="3">
         <v>4</v>
       </c>
+      <c r="G15" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H15" s="1" t="s">
         <v>42</v>
       </c>
@@ -2448,6 +2475,9 @@
       <c r="F16" s="3">
         <v>4</v>
       </c>
+      <c r="G16" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H16" s="1" t="s">
         <v>44</v>
       </c>
@@ -2492,6 +2522,9 @@
       <c r="F17" s="3">
         <v>4</v>
       </c>
+      <c r="G17" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H17" s="1" t="s">
         <v>46</v>
       </c>
@@ -2522,6 +2555,9 @@
         <v>22</v>
       </c>
       <c r="D18" s="3"/>
+      <c r="G18" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H18" s="1" t="s">
         <v>48</v>
       </c>
@@ -2566,6 +2602,9 @@
       <c r="F19" s="3">
         <v>4</v>
       </c>
+      <c r="G19" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H19" s="1" t="s">
         <v>49</v>
       </c>
@@ -3168,6 +3207,9 @@
       <c r="F33" s="3">
         <v>4</v>
       </c>
+      <c r="G33" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H33" s="1" t="s">
         <v>77</v>
       </c>
@@ -3206,6 +3248,9 @@
       <c r="F34" s="3">
         <v>2</v>
       </c>
+      <c r="G34" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H34" s="1" t="s">
         <v>79</v>
       </c>
@@ -3250,6 +3295,9 @@
       <c r="F35" s="3">
         <v>4</v>
       </c>
+      <c r="G35" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H35" s="1" t="s">
         <v>81</v>
       </c>
@@ -3285,6 +3333,9 @@
       <c r="F36" s="3">
         <v>1</v>
       </c>
+      <c r="G36" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H36" s="1" t="s">
         <v>83</v>
       </c>
@@ -3320,6 +3371,9 @@
       <c r="F37" s="3">
         <v>1</v>
       </c>
+      <c r="G37" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H37" s="1" t="s">
         <v>87</v>
       </c>
@@ -3355,6 +3409,9 @@
       <c r="F38" s="3">
         <v>1</v>
       </c>
+      <c r="G38" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H38" s="1" t="s">
         <v>89</v>
       </c>
@@ -3484,7 +3541,7 @@
         <v>317</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>269</v>
+        <v>316</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>112</v>
@@ -3528,7 +3585,7 @@
         <v>317</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>269</v>
+        <v>316</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>114</v>
@@ -3559,6 +3616,9 @@
       <c r="A44" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="G44" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H44" s="1" t="s">
         <v>313</v>
       </c>
@@ -3594,6 +3654,9 @@
       <c r="F45" s="3">
         <v>1</v>
       </c>
+      <c r="G45" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H45" s="1" t="s">
         <v>116</v>
       </c>
@@ -3623,9 +3686,6 @@
       <c r="A46" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G46" s="1" t="s">
-        <v>269</v>
-      </c>
       <c r="H46" s="1" t="s">
         <v>118</v>
       </c>
@@ -3684,6 +3744,9 @@
       <c r="A48" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="G48" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H48" s="1" t="s">
         <v>292</v>
       </c>
@@ -3742,6 +3805,9 @@
       <c r="A50" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="G50" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H50" s="1" t="s">
         <v>102</v>
       </c>
@@ -3890,6 +3956,9 @@
       <c r="A55" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="G55" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H55" s="1" t="s">
         <v>125</v>
       </c>
@@ -3934,6 +4003,9 @@
       <c r="F56" s="3">
         <v>4</v>
       </c>
+      <c r="G56" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H56" s="1" t="s">
         <v>129</v>
       </c>
@@ -4136,6 +4208,9 @@
     <row r="63" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A63" s="1" t="s">
         <v>124</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>316</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>145</v>
@@ -4282,6 +4357,9 @@
       <c r="A68" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="G68" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H68" s="1" t="s">
         <v>157</v>
       </c>
@@ -4605,7 +4683,7 @@
         <v>181</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>167</v>
+        <v>319</v>
       </c>
       <c r="K79" s="1">
         <v>2019</v>
@@ -4692,7 +4770,7 @@
         <v>186</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>173</v>
+        <v>320</v>
       </c>
       <c r="K82" s="1">
         <v>2019</v>
@@ -4779,7 +4857,7 @@
         <v>191</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>178</v>
+        <v>321</v>
       </c>
       <c r="K85" s="1">
         <v>2019</v>
@@ -5702,6 +5780,9 @@
     <row r="117" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A117" s="1" t="s">
         <v>124</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>316</v>
       </c>
       <c r="H117" s="1" t="s">
         <v>276</v>
@@ -5761,6 +5842,9 @@
       <c r="A119" s="1" t="s">
         <v>252</v>
       </c>
+      <c r="G119" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H119" s="1" t="s">
         <v>277</v>
       </c>
@@ -5790,6 +5874,9 @@
       <c r="A120" s="1" t="s">
         <v>252</v>
       </c>
+      <c r="G120" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H120" s="1" t="s">
         <v>278</v>
       </c>
@@ -5819,6 +5906,9 @@
       <c r="A121" s="1" t="s">
         <v>252</v>
       </c>
+      <c r="G121" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="H121" s="1" t="s">
         <v>279</v>
       </c>
@@ -5847,6 +5937,9 @@
     <row r="122" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A122" s="1" t="s">
         <v>252</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>316</v>
       </c>
       <c r="H122" s="1" t="s">
         <v>280</v>

</xml_diff>